<commit_message>
Atualiza o arquivo de sinônimos de conferências
</commit_message>
<xml_diff>
--- a/resources/synonyms/conferences_synonyms.xlsx
+++ b/resources/synonyms/conferences_synonyms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leomurta/workspace/perfil/resources/synonyms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113130E4-DD26-0045-AB63-7D0CCB62A90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21514E91-3806-1B43-9650-68CDFB729BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2197" uniqueCount="2173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2198" uniqueCount="2174">
   <si>
     <t>ACM INTERNATIONAL CONFERENCE ON INTELLIGENT AGENT TECHNOLOGY (IAT)</t>
   </si>
@@ -6539,6 +6539,9 @@
   </si>
   <si>
     <t>SBGAMES - BRAZILIAN SYMPOSIUM ON COMPUTER GAMES AND DIGITAL ENTERTAINMENT</t>
+  </si>
+  <si>
+    <t>20TH IFIP TC13 INTERNATIONAL CONFERENCE ON HUMAN-COMPUTER INTERACTION</t>
   </si>
 </sst>
 </file>
@@ -6904,8 +6907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DF444"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="K183" sqref="K183"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="J120" sqref="J120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9444,6 +9447,9 @@
       <c r="I120" t="s">
         <v>648</v>
       </c>
+      <c r="J120" t="s">
+        <v>2173</v>
+      </c>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">

</xml_diff>